<commit_message>
Cleaned up, export SVGs for report
- moved all library calls to 0- Load common
- created Metadata/labels_NUTS.csv, loaded with other common labels
- commented a few code blocks
- export plots differently: report version without titles and caption
</commit_message>
<xml_diff>
--- a/Tables/Telework_EU.xlsx
+++ b/Tables/Telework_EU.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -365,12 +365,17 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>n_people</t>
+          <t>Person mainly works at home</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>telework_share</t>
+          <t>Person sometimes works at home</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Person never works at home</t>
         </is>
       </c>
     </row>
@@ -379,10 +384,13 @@
         <v>2018</v>
       </c>
       <c r="B2">
-        <v>26795.45703505515</v>
+        <v>10403.09735488775</v>
       </c>
       <c r="C2">
-        <v>0.1372073853792083</v>
+        <v>16392.3596801674</v>
+      </c>
+      <c r="D2">
+        <v>168496.1955315974</v>
       </c>
     </row>
     <row r="3">
@@ -390,10 +398,13 @@
         <v>2019</v>
       </c>
       <c r="B3">
-        <v>28785.91154952973</v>
+        <v>10993.74857470999</v>
       </c>
       <c r="C3">
-        <v>0.1458716886424644</v>
+        <v>17792.16297481974</v>
+      </c>
+      <c r="D3">
+        <v>168551.294987407</v>
       </c>
     </row>
     <row r="4">
@@ -401,10 +412,13 @@
         <v>2020</v>
       </c>
       <c r="B4">
-        <v>40341.08084044303</v>
+        <v>23656.05514102464</v>
       </c>
       <c r="C4">
-        <v>0.2078619292974659</v>
+        <v>16685.02569941839</v>
+      </c>
+      <c r="D4">
+        <v>153735.2513517399</v>
       </c>
     </row>
     <row r="5">
@@ -412,10 +426,13 @@
         <v>2021</v>
       </c>
       <c r="B5">
-        <v>47433.78373301378</v>
+        <v>26551.27259138576</v>
       </c>
       <c r="C5">
-        <v>0.2423428312303083</v>
+        <v>20882.51114162803</v>
+      </c>
+      <c r="D5">
+        <v>148296.3044738683</v>
       </c>
     </row>
     <row r="6">
@@ -423,10 +440,13 @@
         <v>2022</v>
       </c>
       <c r="B6">
-        <v>45334.11712500453</v>
+        <v>20706.19252224476</v>
       </c>
       <c r="C6">
-        <v>0.2259724991892842</v>
+        <v>24627.92460275977</v>
+      </c>
+      <c r="D6">
+        <v>155283.733665019</v>
       </c>
     </row>
   </sheetData>

</xml_diff>